<commit_message>
N and P of feed is now included
</commit_message>
<xml_diff>
--- a/United-States-Canadian-Tables-of-Feed-1982-pages-68-921-with_CrudeProtein.xlsx
+++ b/United-States-Canadian-Tables-of-Feed-1982-pages-68-921-with_CrudeProtein.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6149" uniqueCount="1095">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6149" uniqueCount="1096">
   <si>
     <t>TABLE 2 Composition of Important Feeds: Mineral Elements, Data Expressed As-Fed and Dry (100% Dry Matter)</t>
   </si>
@@ -4700,6 +4700,9 @@
   </si>
   <si>
     <t>BERMUDAGRASS,</t>
+  </si>
+  <si>
+    <t>Entry Number</t>
   </si>
 </sst>
 </file>
@@ -4994,20 +4997,20 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5316,15 +5319,15 @@
   <dimension ref="A1:T1407"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C895" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C766" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S899" sqref="S899"/>
+      <selection pane="bottomRight" activeCell="B764" sqref="B764"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="3.81640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11" style="3" customWidth="1"/>
     <col min="2" max="2" width="13.1796875" customWidth="1"/>
     <col min="3" max="3" width="6.81640625" style="62" customWidth="1"/>
     <col min="4" max="4" width="5" style="10" bestFit="1" customWidth="1"/>
@@ -5362,7 +5365,7 @@
     </row>
     <row r="2" spans="1:20" ht="44" x14ac:dyDescent="0.75">
       <c r="A2" s="14" t="s">
-        <v>2</v>
+        <v>1095</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>1</v>
@@ -9147,10 +9150,10 @@
     </row>
     <row r="80" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A80" s="2"/>
-      <c r="B80" s="68" t="s">
+      <c r="B80" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="C80" s="68"/>
+      <c r="C80" s="70"/>
       <c r="D80" s="11"/>
       <c r="E80" s="12"/>
       <c r="F80" s="12"/>
@@ -11527,10 +11530,10 @@
     </row>
     <row r="142" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A142" s="20"/>
-      <c r="B142" s="69" t="s">
+      <c r="B142" s="68" t="s">
         <v>132</v>
       </c>
-      <c r="C142" s="69"/>
+      <c r="C142" s="68"/>
       <c r="D142" s="21"/>
       <c r="E142" s="22"/>
       <c r="F142" s="22"/>
@@ -11550,11 +11553,11 @@
     </row>
     <row r="143" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A143" s="20"/>
-      <c r="B143" s="70" t="s">
+      <c r="B143" s="69" t="s">
         <v>133</v>
       </c>
-      <c r="C143" s="70"/>
-      <c r="D143" s="70"/>
+      <c r="C143" s="69"/>
+      <c r="D143" s="69"/>
       <c r="E143" s="22"/>
       <c r="F143" s="22"/>
       <c r="G143" s="22"/>
@@ -14473,10 +14476,10 @@
     </row>
     <row r="212" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A212" s="20"/>
-      <c r="B212" s="69" t="s">
+      <c r="B212" s="68" t="s">
         <v>180</v>
       </c>
-      <c r="C212" s="69"/>
+      <c r="C212" s="68"/>
       <c r="D212" s="21"/>
       <c r="E212" s="22"/>
       <c r="F212" s="22"/>
@@ -14496,11 +14499,11 @@
     </row>
     <row r="213" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A213" s="20"/>
-      <c r="B213" s="70" t="s">
+      <c r="B213" s="69" t="s">
         <v>181</v>
       </c>
-      <c r="C213" s="70"/>
-      <c r="D213" s="70"/>
+      <c r="C213" s="69"/>
+      <c r="D213" s="69"/>
       <c r="E213" s="22"/>
       <c r="F213" s="22"/>
       <c r="G213" s="22"/>
@@ -26843,10 +26846,10 @@
     </row>
     <row r="503" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A503" s="2"/>
-      <c r="B503" s="69" t="s">
+      <c r="B503" s="68" t="s">
         <v>406</v>
       </c>
-      <c r="C503" s="69"/>
+      <c r="C503" s="68"/>
       <c r="D503" s="21"/>
       <c r="E503" s="12"/>
       <c r="F503" s="12"/>
@@ -26866,11 +26869,11 @@
     </row>
     <row r="504" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A504" s="2"/>
-      <c r="B504" s="70" t="s">
+      <c r="B504" s="69" t="s">
         <v>407</v>
       </c>
-      <c r="C504" s="70"/>
-      <c r="D504" s="70"/>
+      <c r="C504" s="69"/>
+      <c r="D504" s="69"/>
       <c r="E504" s="12"/>
       <c r="F504" s="12"/>
       <c r="G504" s="12"/>
@@ -30260,10 +30263,10 @@
     </row>
     <row r="594" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A594" s="2"/>
-      <c r="B594" s="69" t="s">
+      <c r="B594" s="68" t="s">
         <v>459</v>
       </c>
-      <c r="C594" s="69"/>
+      <c r="C594" s="68"/>
       <c r="D594" s="11"/>
       <c r="E594" s="12"/>
       <c r="F594" s="12"/>
@@ -31717,10 +31720,10 @@
     </row>
     <row r="635" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A635" s="2"/>
-      <c r="B635" s="68" t="s">
+      <c r="B635" s="70" t="s">
         <v>479</v>
       </c>
-      <c r="C635" s="68"/>
+      <c r="C635" s="70"/>
       <c r="D635" s="11"/>
       <c r="E635" s="12"/>
       <c r="F635" s="12"/>
@@ -33662,10 +33665,10 @@
     </row>
     <row r="686" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A686" s="2"/>
-      <c r="B686" s="69" t="s">
+      <c r="B686" s="68" t="s">
         <v>507</v>
       </c>
-      <c r="C686" s="69"/>
+      <c r="C686" s="68"/>
       <c r="D686" s="11"/>
       <c r="E686" s="12"/>
       <c r="F686" s="12"/>
@@ -33866,10 +33869,10 @@
     </row>
     <row r="692" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A692" s="2"/>
-      <c r="B692" s="69" t="s">
+      <c r="B692" s="68" t="s">
         <v>511</v>
       </c>
-      <c r="C692" s="69"/>
+      <c r="C692" s="68"/>
       <c r="D692" s="11"/>
       <c r="E692" s="12"/>
       <c r="F692" s="12"/>
@@ -33889,10 +33892,10 @@
     </row>
     <row r="693" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A693" s="2"/>
-      <c r="B693" s="70" t="s">
+      <c r="B693" s="69" t="s">
         <v>181</v>
       </c>
-      <c r="C693" s="70"/>
+      <c r="C693" s="69"/>
       <c r="D693" s="11"/>
       <c r="E693" s="12"/>
       <c r="F693" s="12"/>
@@ -33969,11 +33972,11 @@
     </row>
     <row r="695" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A695" s="2"/>
-      <c r="B695" s="69" t="s">
+      <c r="B695" s="68" t="s">
         <v>512</v>
       </c>
-      <c r="C695" s="69"/>
-      <c r="D695" s="69"/>
+      <c r="C695" s="68"/>
+      <c r="D695" s="68"/>
       <c r="E695" s="30"/>
       <c r="F695" s="30"/>
       <c r="G695" s="30"/>
@@ -34211,10 +34214,10 @@
     </row>
     <row r="703" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A703" s="2"/>
-      <c r="B703" s="69" t="s">
+      <c r="B703" s="68" t="s">
         <v>516</v>
       </c>
-      <c r="C703" s="69"/>
+      <c r="C703" s="68"/>
       <c r="D703" s="11"/>
       <c r="E703" s="12"/>
       <c r="F703" s="12"/>
@@ -34234,13 +34237,13 @@
     </row>
     <row r="704" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A704" s="2"/>
-      <c r="B704" s="70" t="s">
+      <c r="B704" s="69" t="s">
         <v>517</v>
       </c>
-      <c r="C704" s="70"/>
-      <c r="D704" s="70"/>
-      <c r="E704" s="70"/>
-      <c r="F704" s="70"/>
+      <c r="C704" s="69"/>
+      <c r="D704" s="69"/>
+      <c r="E704" s="69"/>
+      <c r="F704" s="69"/>
       <c r="G704" s="12"/>
       <c r="H704" s="12"/>
       <c r="I704" s="12"/>
@@ -34278,10 +34281,10 @@
     </row>
     <row r="706" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A706" s="2"/>
-      <c r="B706" s="69" t="s">
+      <c r="B706" s="68" t="s">
         <v>518</v>
       </c>
-      <c r="C706" s="69"/>
+      <c r="C706" s="68"/>
       <c r="D706" s="11"/>
       <c r="E706" s="12"/>
       <c r="F706" s="12"/>
@@ -34301,13 +34304,13 @@
     </row>
     <row r="707" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A707" s="2"/>
-      <c r="B707" s="70" t="s">
+      <c r="B707" s="69" t="s">
         <v>519</v>
       </c>
-      <c r="C707" s="70"/>
-      <c r="D707" s="70"/>
-      <c r="E707" s="70"/>
-      <c r="F707" s="70"/>
+      <c r="C707" s="69"/>
+      <c r="D707" s="69"/>
+      <c r="E707" s="69"/>
+      <c r="F707" s="69"/>
       <c r="G707" s="12"/>
       <c r="H707" s="12"/>
       <c r="I707" s="12"/>
@@ -34345,10 +34348,10 @@
     </row>
     <row r="709" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A709" s="2"/>
-      <c r="B709" s="69" t="s">
+      <c r="B709" s="68" t="s">
         <v>520</v>
       </c>
-      <c r="C709" s="69"/>
+      <c r="C709" s="68"/>
       <c r="D709" s="11"/>
       <c r="E709" s="12"/>
       <c r="F709" s="12"/>
@@ -34368,13 +34371,13 @@
     </row>
     <row r="710" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A710" s="2"/>
-      <c r="B710" s="70" t="s">
+      <c r="B710" s="69" t="s">
         <v>1030</v>
       </c>
-      <c r="C710" s="70"/>
-      <c r="D710" s="70"/>
-      <c r="E710" s="70"/>
-      <c r="F710" s="70"/>
+      <c r="C710" s="69"/>
+      <c r="D710" s="69"/>
+      <c r="E710" s="69"/>
+      <c r="F710" s="69"/>
       <c r="G710" s="12"/>
       <c r="H710" s="12"/>
       <c r="I710" s="12"/>
@@ -34667,10 +34670,10 @@
     </row>
     <row r="717" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A717" s="2"/>
-      <c r="B717" s="69" t="s">
+      <c r="B717" s="68" t="s">
         <v>524</v>
       </c>
-      <c r="C717" s="69"/>
+      <c r="C717" s="68"/>
       <c r="D717" s="11"/>
       <c r="E717" s="12"/>
       <c r="F717" s="12"/>
@@ -34690,13 +34693,13 @@
     </row>
     <row r="718" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A718" s="2"/>
-      <c r="B718" s="70" t="s">
+      <c r="B718" s="69" t="s">
         <v>525</v>
       </c>
-      <c r="C718" s="70"/>
-      <c r="D718" s="70"/>
-      <c r="E718" s="70"/>
-      <c r="F718" s="70"/>
+      <c r="C718" s="69"/>
+      <c r="D718" s="69"/>
+      <c r="E718" s="69"/>
+      <c r="F718" s="69"/>
       <c r="G718" s="12"/>
       <c r="H718" s="12"/>
       <c r="I718" s="12"/>
@@ -34713,14 +34716,14 @@
     </row>
     <row r="719" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A719" s="2"/>
-      <c r="B719" s="68" t="s">
+      <c r="B719" s="70" t="s">
         <v>526</v>
       </c>
-      <c r="C719" s="68"/>
-      <c r="D719" s="68"/>
-      <c r="E719" s="68"/>
-      <c r="F719" s="68"/>
-      <c r="G719" s="68"/>
+      <c r="C719" s="70"/>
+      <c r="D719" s="70"/>
+      <c r="E719" s="70"/>
+      <c r="F719" s="70"/>
+      <c r="G719" s="70"/>
       <c r="H719" s="12"/>
       <c r="I719" s="12"/>
       <c r="J719" s="12"/>
@@ -35632,10 +35635,10 @@
     </row>
     <row r="742" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A742" s="2"/>
-      <c r="B742" s="70" t="s">
+      <c r="B742" s="69" t="s">
         <v>538</v>
       </c>
-      <c r="C742" s="70"/>
+      <c r="C742" s="69"/>
       <c r="D742" s="11"/>
       <c r="E742" s="12"/>
       <c r="F742" s="12"/>
@@ -35790,10 +35793,10 @@
     </row>
     <row r="746" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A746" s="2"/>
-      <c r="B746" s="69" t="s">
+      <c r="B746" s="68" t="s">
         <v>540</v>
       </c>
-      <c r="C746" s="69"/>
+      <c r="C746" s="68"/>
       <c r="D746" s="35"/>
       <c r="E746" s="12"/>
       <c r="F746" s="12"/>
@@ -35834,11 +35837,11 @@
     </row>
     <row r="748" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A748" s="2"/>
-      <c r="B748" s="69" t="s">
+      <c r="B748" s="68" t="s">
         <v>541</v>
       </c>
-      <c r="C748" s="69"/>
-      <c r="D748" s="69"/>
+      <c r="C748" s="68"/>
+      <c r="D748" s="68"/>
       <c r="E748" s="12"/>
       <c r="F748" s="12"/>
       <c r="G748" s="12"/>
@@ -36028,11 +36031,11 @@
     </row>
     <row r="752" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A752" s="2"/>
-      <c r="B752" s="71" t="s">
+      <c r="B752" s="72" t="s">
         <v>543</v>
       </c>
-      <c r="C752" s="71"/>
-      <c r="D752" s="71"/>
+      <c r="C752" s="72"/>
+      <c r="D752" s="72"/>
       <c r="E752" s="30"/>
       <c r="F752" s="30"/>
       <c r="G752" s="30"/>
@@ -36072,11 +36075,11 @@
     </row>
     <row r="754" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A754" s="2"/>
-      <c r="B754" s="71" t="s">
+      <c r="B754" s="72" t="s">
         <v>544</v>
       </c>
-      <c r="C754" s="71"/>
-      <c r="D754" s="71"/>
+      <c r="C754" s="72"/>
+      <c r="D754" s="72"/>
       <c r="E754" s="30"/>
       <c r="F754" s="30"/>
       <c r="G754" s="30"/>
@@ -36116,12 +36119,12 @@
     </row>
     <row r="756" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A756" s="2"/>
-      <c r="B756" s="71" t="s">
+      <c r="B756" s="72" t="s">
         <v>545</v>
       </c>
-      <c r="C756" s="71"/>
-      <c r="D756" s="71"/>
-      <c r="E756" s="71"/>
+      <c r="C756" s="72"/>
+      <c r="D756" s="72"/>
+      <c r="E756" s="72"/>
       <c r="F756" s="30"/>
       <c r="G756" s="30"/>
       <c r="H756" s="30"/>
@@ -36160,14 +36163,14 @@
     </row>
     <row r="758" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A758" s="2"/>
-      <c r="B758" s="71" t="s">
+      <c r="B758" s="72" t="s">
         <v>546</v>
       </c>
-      <c r="C758" s="71"/>
-      <c r="D758" s="71"/>
-      <c r="E758" s="71"/>
-      <c r="F758" s="71"/>
-      <c r="G758" s="71"/>
+      <c r="C758" s="72"/>
+      <c r="D758" s="72"/>
+      <c r="E758" s="72"/>
+      <c r="F758" s="72"/>
+      <c r="G758" s="72"/>
       <c r="H758" s="30"/>
       <c r="I758" s="30"/>
       <c r="J758" s="30"/>
@@ -36204,14 +36207,14 @@
     </row>
     <row r="760" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A760" s="2"/>
-      <c r="B760" s="71" t="s">
+      <c r="B760" s="72" t="s">
         <v>547</v>
       </c>
-      <c r="C760" s="71"/>
-      <c r="D760" s="71"/>
-      <c r="E760" s="71"/>
-      <c r="F760" s="71"/>
-      <c r="G760" s="71"/>
+      <c r="C760" s="72"/>
+      <c r="D760" s="72"/>
+      <c r="E760" s="72"/>
+      <c r="F760" s="72"/>
+      <c r="G760" s="72"/>
       <c r="H760" s="30"/>
       <c r="I760" s="30"/>
       <c r="J760" s="30"/>
@@ -38365,9 +38368,9 @@
     </row>
     <row r="811" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A811" s="2"/>
-      <c r="B811" s="69"/>
-      <c r="C811" s="69"/>
-      <c r="D811" s="69"/>
+      <c r="B811" s="68"/>
+      <c r="C811" s="68"/>
+      <c r="D811" s="68"/>
       <c r="E811" s="30"/>
       <c r="F811" s="30"/>
       <c r="G811" s="30"/>
@@ -46383,10 +46386,10 @@
     </row>
     <row r="999" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A999" s="2"/>
-      <c r="B999" s="72" t="s">
+      <c r="B999" s="71" t="s">
         <v>724</v>
       </c>
-      <c r="C999" s="72"/>
+      <c r="C999" s="71"/>
       <c r="D999" s="11"/>
       <c r="E999" s="12"/>
       <c r="F999" s="12"/>
@@ -50401,11 +50404,11 @@
     </row>
     <row r="1097" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1097" s="2"/>
-      <c r="B1097" s="69" t="s">
+      <c r="B1097" s="68" t="s">
         <v>786</v>
       </c>
-      <c r="C1097" s="69"/>
-      <c r="D1097" s="69"/>
+      <c r="C1097" s="68"/>
+      <c r="D1097" s="68"/>
       <c r="E1097" s="30"/>
       <c r="F1097" s="30"/>
       <c r="G1097" s="30"/>
@@ -50424,11 +50427,11 @@
     </row>
     <row r="1098" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1098" s="2"/>
-      <c r="B1098" s="70" t="s">
+      <c r="B1098" s="69" t="s">
         <v>787</v>
       </c>
-      <c r="C1098" s="70"/>
-      <c r="D1098" s="70"/>
+      <c r="C1098" s="69"/>
+      <c r="D1098" s="69"/>
       <c r="E1098" s="30"/>
       <c r="F1098" s="30"/>
       <c r="G1098" s="30"/>
@@ -52394,10 +52397,10 @@
     </row>
     <row r="1148" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1148" s="2"/>
-      <c r="B1148" s="69" t="s">
+      <c r="B1148" s="68" t="s">
         <v>812</v>
       </c>
-      <c r="C1148" s="69"/>
+      <c r="C1148" s="68"/>
       <c r="D1148" s="11"/>
       <c r="E1148" s="12"/>
       <c r="F1148" s="12"/>
@@ -52634,11 +52637,11 @@
     </row>
     <row r="1154" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1154" s="2"/>
-      <c r="B1154" s="69" t="s">
+      <c r="B1154" s="68" t="s">
         <v>816</v>
       </c>
-      <c r="C1154" s="69"/>
-      <c r="D1154" s="69"/>
+      <c r="C1154" s="68"/>
+      <c r="D1154" s="68"/>
       <c r="E1154" s="30"/>
       <c r="F1154" s="30"/>
       <c r="G1154" s="30"/>
@@ -55104,11 +55107,11 @@
     </row>
     <row r="1208" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1208" s="2"/>
-      <c r="B1208" s="69" t="s">
+      <c r="B1208" s="68" t="s">
         <v>854</v>
       </c>
-      <c r="C1208" s="69"/>
-      <c r="D1208" s="69"/>
+      <c r="C1208" s="68"/>
+      <c r="D1208" s="68"/>
       <c r="E1208" s="12"/>
       <c r="F1208" s="12"/>
       <c r="G1208" s="12"/>
@@ -55207,11 +55210,11 @@
     </row>
     <row r="1211" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1211" s="2"/>
-      <c r="B1211" s="69" t="s">
+      <c r="B1211" s="68" t="s">
         <v>1062</v>
       </c>
-      <c r="C1211" s="69"/>
-      <c r="D1211" s="69"/>
+      <c r="C1211" s="68"/>
+      <c r="D1211" s="68"/>
       <c r="E1211" s="30"/>
       <c r="F1211" s="30"/>
       <c r="G1211" s="30"/>
@@ -55230,10 +55233,10 @@
     </row>
     <row r="1212" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1212" s="2"/>
-      <c r="B1212" s="68" t="s">
+      <c r="B1212" s="70" t="s">
         <v>856</v>
       </c>
-      <c r="C1212" s="68"/>
+      <c r="C1212" s="70"/>
       <c r="D1212" s="26"/>
       <c r="E1212" s="30"/>
       <c r="F1212" s="30"/>
@@ -57746,11 +57749,11 @@
     </row>
     <row r="1270" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1270" s="2"/>
-      <c r="B1270" s="69" t="s">
+      <c r="B1270" s="68" t="s">
         <v>887</v>
       </c>
-      <c r="C1270" s="69"/>
-      <c r="D1270" s="69"/>
+      <c r="C1270" s="68"/>
+      <c r="D1270" s="68"/>
       <c r="E1270" s="30"/>
       <c r="F1270" s="30"/>
       <c r="G1270" s="30"/>
@@ -57769,10 +57772,10 @@
     </row>
     <row r="1271" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1271" s="2"/>
-      <c r="B1271" s="70" t="s">
+      <c r="B1271" s="69" t="s">
         <v>888</v>
       </c>
-      <c r="C1271" s="70"/>
+      <c r="C1271" s="69"/>
       <c r="D1271" s="26"/>
       <c r="E1271" s="30"/>
       <c r="F1271" s="30"/>
@@ -59998,9 +60001,9 @@
     </row>
     <row r="1328" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1328" s="2"/>
-      <c r="B1328" s="69"/>
-      <c r="C1328" s="69"/>
-      <c r="D1328" s="69"/>
+      <c r="B1328" s="68"/>
+      <c r="C1328" s="68"/>
+      <c r="D1328" s="68"/>
       <c r="E1328" s="30"/>
       <c r="F1328" s="30"/>
       <c r="G1328" s="30"/>
@@ -63064,10 +63067,10 @@
     </row>
     <row r="1392" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1392" s="2"/>
-      <c r="B1392" s="69" t="s">
+      <c r="B1392" s="68" t="s">
         <v>974</v>
       </c>
-      <c r="C1392" s="69"/>
+      <c r="C1392" s="68"/>
       <c r="D1392" s="11"/>
       <c r="E1392" s="12"/>
       <c r="F1392" s="12"/>
@@ -63087,10 +63090,10 @@
     </row>
     <row r="1393" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1393" s="2"/>
-      <c r="B1393" s="70" t="s">
+      <c r="B1393" s="69" t="s">
         <v>975</v>
       </c>
-      <c r="C1393" s="70"/>
+      <c r="C1393" s="69"/>
       <c r="D1393" s="11"/>
       <c r="E1393" s="12"/>
       <c r="F1393" s="12"/>
@@ -63700,6 +63703,41 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="B143:D143"/>
+    <mergeCell ref="B212:C212"/>
+    <mergeCell ref="B213:D213"/>
+    <mergeCell ref="B503:C503"/>
+    <mergeCell ref="B504:D504"/>
+    <mergeCell ref="B594:C594"/>
+    <mergeCell ref="B635:C635"/>
+    <mergeCell ref="B686:C686"/>
+    <mergeCell ref="B692:C692"/>
+    <mergeCell ref="B693:C693"/>
+    <mergeCell ref="B695:D695"/>
+    <mergeCell ref="B703:C703"/>
+    <mergeCell ref="B704:F704"/>
+    <mergeCell ref="B706:C706"/>
+    <mergeCell ref="B707:F707"/>
+    <mergeCell ref="B709:C709"/>
+    <mergeCell ref="B710:F710"/>
+    <mergeCell ref="B717:C717"/>
+    <mergeCell ref="B718:F718"/>
+    <mergeCell ref="B719:G719"/>
+    <mergeCell ref="B742:C742"/>
+    <mergeCell ref="B746:C746"/>
+    <mergeCell ref="B748:D748"/>
+    <mergeCell ref="B752:D752"/>
+    <mergeCell ref="B754:D754"/>
+    <mergeCell ref="B756:E756"/>
+    <mergeCell ref="B758:G758"/>
+    <mergeCell ref="B760:G760"/>
+    <mergeCell ref="B811:D811"/>
+    <mergeCell ref="B999:C999"/>
+    <mergeCell ref="B1097:D1097"/>
+    <mergeCell ref="B1098:D1098"/>
+    <mergeCell ref="B1148:C1148"/>
     <mergeCell ref="B1154:D1154"/>
     <mergeCell ref="B1208:D1208"/>
     <mergeCell ref="B1211:D1211"/>
@@ -63709,41 +63747,6 @@
     <mergeCell ref="B1271:C1271"/>
     <mergeCell ref="B1328:D1328"/>
     <mergeCell ref="B1392:C1392"/>
-    <mergeCell ref="B811:D811"/>
-    <mergeCell ref="B999:C999"/>
-    <mergeCell ref="B1097:D1097"/>
-    <mergeCell ref="B1098:D1098"/>
-    <mergeCell ref="B1148:C1148"/>
-    <mergeCell ref="B752:D752"/>
-    <mergeCell ref="B754:D754"/>
-    <mergeCell ref="B756:E756"/>
-    <mergeCell ref="B758:G758"/>
-    <mergeCell ref="B760:G760"/>
-    <mergeCell ref="B718:F718"/>
-    <mergeCell ref="B719:G719"/>
-    <mergeCell ref="B742:C742"/>
-    <mergeCell ref="B746:C746"/>
-    <mergeCell ref="B748:D748"/>
-    <mergeCell ref="B706:C706"/>
-    <mergeCell ref="B707:F707"/>
-    <mergeCell ref="B709:C709"/>
-    <mergeCell ref="B710:F710"/>
-    <mergeCell ref="B717:C717"/>
-    <mergeCell ref="B692:C692"/>
-    <mergeCell ref="B693:C693"/>
-    <mergeCell ref="B695:D695"/>
-    <mergeCell ref="B703:C703"/>
-    <mergeCell ref="B704:F704"/>
-    <mergeCell ref="B503:C503"/>
-    <mergeCell ref="B504:D504"/>
-    <mergeCell ref="B594:C594"/>
-    <mergeCell ref="B635:C635"/>
-    <mergeCell ref="B686:C686"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B142:C142"/>
-    <mergeCell ref="B143:D143"/>
-    <mergeCell ref="B212:C212"/>
-    <mergeCell ref="B213:D213"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" firstPageNumber="59" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>